<commit_message>
add SWB code on ukb
</commit_message>
<xml_diff>
--- a/construction/rGSES_top_phenotypes.xlsx
+++ b/construction/rGSES_top_phenotypes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\econ\biroli\geighei\code\GWAS_cleaning\GWAS_construction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parce\Desktop\GeiGhei\GWAS_cleaning\construction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4CBA94-6976-4D75-9166-8F1B37CB51AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC45DE9-22D7-45FE-B9EB-27505EC85A0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BE44C88F-6FBC-0744-BA82-1F47EBF5319D}"/>
   </bookViews>
@@ -468,7 +468,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -496,6 +496,12 @@
       <sz val="14"/>
       <color rgb="FF333333"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -593,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -606,6 +612,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -926,13 +933,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212B4500-157A-D94A-987F-740F8575CE4A}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31:K48"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.25" customWidth="1"/>
     <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.1640625" bestFit="1" customWidth="1"/>
@@ -1515,7 +1522,9 @@
       <c r="G22">
         <v>19</v>
       </c>
-      <c r="J22" s="9"/>
+      <c r="J22" s="12">
+        <v>4526</v>
+      </c>
       <c r="K22" t="s">
         <v>121</v>
       </c>
@@ -2194,5 +2203,6 @@
     <hyperlink ref="J34" r:id="rId4" display="http://biobank.ctsu.ox.ac.uk/crystal/field.cgi?id=2946" xr:uid="{0D701672-B2BE-44F5-9E02-B9B68C684CFE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding ischemic heart disease as CAD
</commit_message>
<xml_diff>
--- a/construction/rGSES_top_phenotypes.xlsx
+++ b/construction/rGSES_top_phenotypes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parce\Desktop\GeiGhei\GWAS_cleaning\construction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E970FF38-72E5-4496-B592-B5B8CCEE9A3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95ACA5F0-A507-49F5-93B6-0747828084EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BE44C88F-6FBC-0744-BA82-1F47EBF5319D}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="137">
   <si>
     <t xml:space="preserve">Variables </t>
   </si>
@@ -933,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212B4500-157A-D94A-987F-740F8575CE4A}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
@@ -1324,7 +1324,12 @@
       <c r="G14">
         <v>11</v>
       </c>
-      <c r="J14" s="9"/>
+      <c r="I14" t="s">
+        <v>136</v>
+      </c>
+      <c r="J14" s="9">
+        <v>41204</v>
+      </c>
       <c r="K14" t="s">
         <v>115</v>
       </c>
@@ -1535,6 +1540,7 @@
       <c r="G22">
         <v>19</v>
       </c>
+      <c r="I22" s="12"/>
       <c r="J22" s="12">
         <v>4526</v>
       </c>

</xml_diff>